<commit_message>
PC increment bug fixed, mipsInstructions spaced to word align
</commit_message>
<xml_diff>
--- a/3rd/Control.xlsx
+++ b/3rd/Control.xlsx
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1117,7 @@
         <v>00000001100000</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="N30:O38" si="3">BIN2HEX(VALUE(N30))</f>
+        <f t="shared" ref="O30:O38" si="3">BIN2HEX(VALUE(N30))</f>
         <v>60</v>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -1408,11 +1408,11 @@
       </c>
       <c r="N36" t="str">
         <f t="shared" si="2"/>
-        <v>00000000011001</v>
+        <v>00000000010001</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>